<commit_message>
fixed bug in category_to_sector share & vignette work
</commit_message>
<xml_diff>
--- a/inst/extdata/master-implan-sectoring536.xlsx
+++ b/inst/extdata/master-implan-sectoring536.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SA\Project\_R_packages\implan\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB62023D-8E77-46BF-8A16-2820EDC8E9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651599A8-66C2-4449-B7FE-C688E11DC1B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="1050" windowWidth="24240" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="293">
   <si>
     <t>See report:</t>
   </si>
@@ -909,6 +909,9 @@
   </si>
   <si>
     <t>Will need to make some changes to the "Retail" column (from "Yes" to "No") for the new Implan 546 to avoid margin setting errors</t>
+  </si>
+  <si>
+    <t>Blue-highlighted cells had issues with share sums by category</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -965,6 +968,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1010,6 +1019,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,10 +1319,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,23 +1397,28 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>288</v>
       </c>
     </row>
@@ -1418,11 +1433,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5E2F36-A4A9-472A-8E5E-5252E07535B0}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,6 +2334,126 @@
         <v>22</v>
       </c>
     </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38">
+        <v>494</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0.1959722585</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39">
+        <v>495</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="11">
+        <v>0.3040277415</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40">
+        <v>496</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>250</v>
+      </c>
+      <c r="C41">
+        <v>523</v>
+      </c>
+      <c r="D41" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41">
+        <v>0.5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>250</v>
+      </c>
+      <c r="C42">
+        <v>531</v>
+      </c>
+      <c r="D42" t="s">
+        <v>251</v>
+      </c>
+      <c r="E42">
+        <v>0.169874405663171</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43">
+        <v>533</v>
+      </c>
+      <c r="D43" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43">
+        <v>0.33012559433682898</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
     <sortCondition ref="B2:B37"/>
@@ -2334,8 +2469,8 @@
   <dimension ref="A1:I248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A214" sqref="A214:F216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>